<commit_message>
I added some writing
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/test/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/test/Data-Squad/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,6 +24,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>asldfkj</t>
+  </si>
+  <si>
+    <t>saldjf</t>
+  </si>
+  <si>
+    <t>asdlkfj</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +350,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D8:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="8" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "said hi""
This reverts commit 6a55d86dbbf381720c698e7a3f6cb4f5ec6bc84d.
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>asldfkj</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>asdlkfj</t>
+  </si>
+  <si>
+    <t>Hello Canada</t>
   </si>
 </sst>
 </file>
@@ -350,25 +353,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D8:D13"/>
+  <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>2</v>
       </c>

</xml_diff>